<commit_message>
update business logic @Author : Alex
</commit_message>
<xml_diff>
--- a/02 Detail Design/数据库设计书.xlsx
+++ b/02 Detail Design/数据库设计书.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20475" windowHeight="7845" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20475" windowHeight="7845" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Risk 分类和举例" sheetId="1" state="hidden" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="354">
   <si>
     <t>风险分类</t>
   </si>
@@ -1698,6 +1698,18 @@
   <si>
     <t>依据中兴多渠道下载技术提案修改打包信息表</t>
     <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>排位顺序</t>
+  </si>
+  <si>
+    <t>SORT</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>前30游戏的排位顺序</t>
   </si>
 </sst>
 </file>
@@ -6675,7 +6687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
@@ -7901,7 +7913,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="T25" sqref="T24:T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8130,7 +8142,7 @@
         <v>311</v>
       </c>
       <c r="I9" s="43">
-        <v>50</v>
+        <v>128</v>
       </c>
       <c r="J9" s="43"/>
       <c r="K9" s="43" t="s">
@@ -11855,10 +11867,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18:O18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
@@ -12039,7 +12051,7 @@
     <row r="8" spans="1:15">
       <c r="A8" s="2"/>
       <c r="B8" s="42">
-        <f t="shared" ref="B8:B26" si="0">ROW()-6</f>
+        <f t="shared" ref="B8:B28" si="0">ROW()-6</f>
         <v>2</v>
       </c>
       <c r="C8" s="42"/>
@@ -12104,7 +12116,7 @@
       <c r="N9" s="127"/>
       <c r="O9" s="128"/>
     </row>
-    <row r="10" spans="1:15" ht="22.5">
+    <row r="10" spans="1:15">
       <c r="A10" s="2"/>
       <c r="B10" s="42">
         <f t="shared" si="0"/>
@@ -12114,13 +12126,13 @@
       <c r="D10" s="42"/>
       <c r="E10" s="42"/>
       <c r="F10" s="43" t="s">
-        <v>156</v>
+        <v>350</v>
       </c>
       <c r="G10" s="43" t="s">
-        <v>157</v>
+        <v>351</v>
       </c>
       <c r="H10" s="43" t="s">
-        <v>145</v>
+        <v>352</v>
       </c>
       <c r="I10" s="43">
         <v>20</v>
@@ -12133,7 +12145,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="126" t="s">
-        <v>180</v>
+        <v>353</v>
       </c>
       <c r="N10" s="127"/>
       <c r="O10" s="128"/>
@@ -12148,25 +12160,31 @@
       <c r="D11" s="42"/>
       <c r="E11" s="42"/>
       <c r="F11" s="43" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="G11" s="43" t="s">
-        <v>277</v>
+        <v>157</v>
       </c>
       <c r="H11" s="43" t="s">
-        <v>296</v>
-      </c>
-      <c r="I11" s="43"/>
+        <v>145</v>
+      </c>
+      <c r="I11" s="43">
+        <v>20</v>
+      </c>
       <c r="J11" s="43"/>
       <c r="K11" s="43" t="s">
         <v>154</v>
       </c>
-      <c r="L11" s="42"/>
-      <c r="M11" s="126"/>
+      <c r="L11" s="42">
+        <v>0</v>
+      </c>
+      <c r="M11" s="126" t="s">
+        <v>180</v>
+      </c>
       <c r="N11" s="127"/>
       <c r="O11" s="128"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" ht="22.5">
       <c r="A12" s="2"/>
       <c r="B12" s="42">
         <f t="shared" si="0"/>
@@ -12176,29 +12194,31 @@
       <c r="D12" s="42"/>
       <c r="E12" s="42"/>
       <c r="F12" s="43" t="s">
-        <v>301</v>
+        <v>177</v>
       </c>
       <c r="G12" s="43" t="s">
-        <v>300</v>
+        <v>178</v>
       </c>
       <c r="H12" s="43" t="s">
-        <v>299</v>
-      </c>
-      <c r="I12" s="43"/>
+        <v>142</v>
+      </c>
+      <c r="I12" s="43">
+        <v>20</v>
+      </c>
       <c r="J12" s="43"/>
       <c r="K12" s="43" t="s">
         <v>154</v>
       </c>
-      <c r="L12" s="42" t="b">
+      <c r="L12" s="42">
         <v>0</v>
       </c>
       <c r="M12" s="126" t="s">
-        <v>302</v>
+        <v>177</v>
       </c>
       <c r="N12" s="127"/>
       <c r="O12" s="128"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" ht="22.5">
       <c r="A13" s="2"/>
       <c r="B13" s="42">
         <f t="shared" si="0"/>
@@ -12207,12 +12227,20 @@
       <c r="C13" s="42"/>
       <c r="D13" s="42"/>
       <c r="E13" s="42"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
+      <c r="F13" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>277</v>
+      </c>
+      <c r="H13" s="43" t="s">
+        <v>296</v>
+      </c>
       <c r="I13" s="43"/>
       <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
+      <c r="K13" s="43" t="s">
+        <v>154</v>
+      </c>
       <c r="L13" s="42"/>
       <c r="M13" s="126"/>
       <c r="N13" s="127"/>
@@ -12227,14 +12255,26 @@
       <c r="C14" s="42"/>
       <c r="D14" s="42"/>
       <c r="E14" s="42"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
+      <c r="F14" s="43" t="s">
+        <v>301</v>
+      </c>
+      <c r="G14" s="43" t="s">
+        <v>300</v>
+      </c>
+      <c r="H14" s="43" t="s">
+        <v>299</v>
+      </c>
       <c r="I14" s="43"/>
       <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="126"/>
+      <c r="K14" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="L14" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="M14" s="126" t="s">
+        <v>302</v>
+      </c>
       <c r="N14" s="127"/>
       <c r="O14" s="128"/>
     </row>
@@ -12288,11 +12328,11 @@
       <c r="D17" s="42"/>
       <c r="E17" s="42"/>
       <c r="F17" s="43"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
       <c r="L17" s="42"/>
       <c r="M17" s="126"/>
       <c r="N17" s="127"/>
@@ -12308,11 +12348,11 @@
       <c r="D18" s="42"/>
       <c r="E18" s="42"/>
       <c r="F18" s="43"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
       <c r="L18" s="42"/>
       <c r="M18" s="126"/>
       <c r="N18" s="127"/>
@@ -12478,30 +12518,72 @@
       <c r="N26" s="127"/>
       <c r="O26" s="128"/>
     </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="2"/>
+      <c r="B27" s="42">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="126"/>
+      <c r="N27" s="127"/>
+      <c r="O27" s="128"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="2"/>
+      <c r="B28" s="42">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="42"/>
+      <c r="M28" s="126"/>
+      <c r="N28" s="127"/>
+      <c r="O28" s="128"/>
+    </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="M16:O16"/>
+  <mergeCells count="24">
+    <mergeCell ref="M18:O18"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="M6:O6"/>
     <mergeCell ref="M7:O7"/>
     <mergeCell ref="M8:O8"/>
     <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M10:O10"/>
     <mergeCell ref="M11:O11"/>
-    <mergeCell ref="M12:O12"/>
     <mergeCell ref="M13:O13"/>
     <mergeCell ref="M14:O14"/>
     <mergeCell ref="M15:O15"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M10:O10"/>
     <mergeCell ref="M25:O25"/>
     <mergeCell ref="M26:O26"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="M28:O28"/>
     <mergeCell ref="M19:O19"/>
     <mergeCell ref="M20:O20"/>
     <mergeCell ref="M21:O21"/>
     <mergeCell ref="M22:O22"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M24:O24"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13152,7 +13234,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F10" sqref="F10:O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="12.75"/>

</xml_diff>